<commit_message>
Added the url address column
Added the column
</commit_message>
<xml_diff>
--- a/documents/PPDM Website Cookies Data-Khan.xlsx
+++ b/documents/PPDM Website Cookies Data-Khan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farah\Documents\GitHub\PPDM_Dev_Prototype_Odoo\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E4BFFB-4681-49CB-98E7-7DAE5828D206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55572260-B2AA-4EC6-BD4A-47C14C59BF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
   <si>
     <t>S No</t>
   </si>
@@ -169,13 +169,58 @@
   </si>
   <si>
     <t>Necessary,Preference,Statistics,MarketingUnclassified,Cross domain consent</t>
+  </si>
+  <si>
+    <t>URL Website</t>
+  </si>
+  <si>
+    <t>https://www.onetrust.com/</t>
+  </si>
+  <si>
+    <t>https://brightbridgesolutions.com/</t>
+  </si>
+  <si>
+    <t>https://www.kellton.com/</t>
+  </si>
+  <si>
+    <t>https://mirus-it.co.uk/</t>
+  </si>
+  <si>
+    <t>https://www.russellreynolds.com/en/</t>
+  </si>
+  <si>
+    <t>https://www.bain.com/offices/london/</t>
+  </si>
+  <si>
+    <t>https://www.itransition.com/</t>
+  </si>
+  <si>
+    <t>https://www.webbytech.co.uk/</t>
+  </si>
+  <si>
+    <t>https://trilan-it.com/</t>
+  </si>
+  <si>
+    <t>https://www.lumen.com/en-us/home.html</t>
+  </si>
+  <si>
+    <t>https://conosco.com/</t>
+  </si>
+  <si>
+    <t>https://www.transparity.com/latest-news/transparity-acquire-microsoft-azure-development-specialist-ballard-chalmers/</t>
+  </si>
+  <si>
+    <t>https://www.ecl.co.uk/</t>
+  </si>
+  <si>
+    <t>https://www.topdesk.com/en/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -198,6 +243,13 @@
       <b/>
       <sz val="18"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -252,10 +304,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -290,8 +343,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -604,380 +661,435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:G17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.453125" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="10.36328125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="43.453125" style="4"/>
-    <col min="3" max="3" width="55.36328125" customWidth="1"/>
+    <col min="2" max="3" width="43.453125" style="4"/>
+    <col min="4" max="4" width="55.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.5">
+    <row r="1" spans="1:8" ht="23.5">
       <c r="A1" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="130.5">
+    <row r="4" spans="1:8" ht="130.5">
       <c r="A4" s="7">
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" ht="130.5">
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" ht="130.5">
       <c r="A5" s="7">
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" ht="72.5">
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" ht="72.5">
       <c r="A6" s="7">
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="7">
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="43.5">
+    <row r="8" spans="1:8" ht="43.5">
       <c r="A8" s="7">
         <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="43.5">
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" ht="43.5">
       <c r="A9" s="7">
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="72.5">
+    <row r="10" spans="1:8" ht="72.5">
       <c r="A10" s="7">
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="D10" s="9"/>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="7">
         <v>8</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="7">
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="9"/>
+      <c r="H12" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="43.5">
+    <row r="13" spans="1:8" ht="43.5">
       <c r="A13" s="7">
         <v>10</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" ht="58">
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" ht="58">
       <c r="A14" s="7">
         <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="9"/>
+      <c r="C14" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="9"/>
+      <c r="H14" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="101.5">
+    <row r="15" spans="1:8" ht="101.5">
       <c r="A15" s="7">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="9"/>
+      <c r="H15" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" s="7">
         <v>13</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="9"/>
+      <c r="H16" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="29">
+    <row r="17" spans="1:8" ht="29">
       <c r="A17" s="7">
         <v>14</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="9"/>
+      <c r="H17" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="2"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
+      <c r="C20" s="2"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="2"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
+      <c r="C22" s="2"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="2"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
+      <c r="C24" s="2"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
+      <c r="C25" s="2"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
First and Third party
Added Firtst and Third party Clients
</commit_message>
<xml_diff>
--- a/documents/PPDM Website Cookies Data-Khan.xlsx
+++ b/documents/PPDM Website Cookies Data-Khan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farah\Documents\GitHub\PPDM_Dev_Prototype_Odoo\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A0A189-B6FF-47BA-AE6C-901AA39D883A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F8F0F1-3203-4074-B8E9-1D9016E605AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
   <si>
     <t>S No</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>Statistics 7 ,Marketing 2 Un classified 2</t>
+  </si>
+  <si>
+    <t>Vendors</t>
+  </si>
+  <si>
+    <t>First Party - Optanon Consent  &amp; AW SalB.. Third Party-  _GRECAPTCHA</t>
   </si>
 </sst>
 </file>
@@ -332,7 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,6 +372,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -685,33 +694,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.453125" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="10.36328125" style="4" customWidth="1"/>
     <col min="2" max="3" width="43.453125" style="4"/>
-    <col min="4" max="4" width="55.36328125" customWidth="1"/>
+    <col min="4" max="5" width="55.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.5">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:9" ht="23.5">
+      <c r="A1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -725,19 +735,22 @@
         <v>2</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="130.5">
+    <row r="4" spans="1:9" ht="130.5">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -751,41 +764,45 @@
         <v>28</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:8" ht="130.5">
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" ht="130.5">
       <c r="A5" s="7">
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="11" t="s">
         <v>51</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" ht="72.5">
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" ht="72.5">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -798,18 +815,19 @@
       <c r="D6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -823,11 +841,12 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.5">
+    <row r="8" spans="1:9" ht="43.5">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -840,18 +859,19 @@
       <c r="D8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" ht="43.5">
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" ht="43.5">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -864,20 +884,21 @@
       <c r="D9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="72.5">
+    <row r="10" spans="1:9" ht="72.5">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -889,15 +910,16 @@
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="9"/>
+      <c r="I10" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -911,11 +933,12 @@
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="9"/>
+      <c r="I11" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -929,11 +952,12 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="9"/>
+      <c r="I12" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="43.5">
+    <row r="13" spans="1:9" ht="43.5">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -946,18 +970,19 @@
       <c r="D13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:8" ht="58">
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" ht="58">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -971,11 +996,12 @@
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="9"/>
+      <c r="I14" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="101.5">
+    <row r="15" spans="1:9" ht="101.5">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -991,11 +1017,12 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="9"/>
+      <c r="I15" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="7">
         <v>13</v>
       </c>
@@ -1009,11 +1036,12 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="9"/>
+      <c r="I16" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="29">
+    <row r="17" spans="1:9" ht="29">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -1027,11 +1055,12 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="9" t="s">
+      <c r="H17" s="9"/>
+      <c r="I17" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="72.5">
+    <row r="18" spans="1:9" ht="72.5">
       <c r="A18" s="7">
         <v>15</v>
       </c>
@@ -1044,16 +1073,17 @@
       <c r="D18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="9"/>
+      <c r="F18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="9"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="9"/>
+      <c r="I18" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9">
       <c r="A19" s="7">
         <v>16</v>
       </c>
@@ -1066,16 +1096,17 @@
       <c r="D19" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="9"/>
+      <c r="F19" s="9">
         <v>0</v>
       </c>
-      <c r="F19" s="9"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="9"/>
+      <c r="I19" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1084,8 +1115,9 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1094,8 +1126,9 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1104,8 +1137,9 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1114,8 +1148,9 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1124,8 +1159,9 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1134,6 +1170,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1142,9 +1179,10 @@
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{4FB45887-2ECC-4325-88AC-1EDA7419751B}"/>
     <hyperlink ref="C19" r:id="rId2" xr:uid="{F6283996-83CC-4B7B-AA3F-CA50AE69AA43}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{FFCBEBCC-0613-4429-840C-185ACAA14A71}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>